<commit_message>
Documentation ready to be checked
</commit_message>
<xml_diff>
--- a/CourseAssignment/burndownChart.xlsx
+++ b/CourseAssignment/burndownChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Claudiu\Desktop\SEP2\SEP2Group\CourseAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2077A6-7FED-425C-BDC0-34DEDF5EFD8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA2A07C-DF32-4EF9-A915-2BFA75A96AB2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{16860CCE-BD4E-434D-99B6-05202FD211FB}"/>
   </bookViews>
@@ -26,12 +26,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Remaining Work</t>
-  </si>
-  <si>
-    <t>Completed Work</t>
-  </si>
   <si>
     <t>Date</t>
   </si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>30/04/2018</t>
+  </si>
+  <si>
+    <t>Ideal Completion</t>
+  </si>
+  <si>
+    <t>Actual Completion</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Remaining Work</c:v>
+                  <c:v>Actual Completion</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -181,7 +181,7 @@
             <c:strRef>
               <c:f>Sheet1!$C$5:$C$18</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>23/04/2018</c:v>
                 </c:pt>
@@ -211,6 +211,9 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2/5/2018</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3/5/2018</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -225,22 +228,34 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -261,7 +276,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Completed Work</c:v>
+                  <c:v>Ideal Completion</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -291,25 +306,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -322,7 +349,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="ctr"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -585,7 +611,7 @@
       </c:valAx>
       <c:spPr>
         <a:noFill/>
-        <a:ln>
+        <a:ln w="25400">
           <a:noFill/>
         </a:ln>
         <a:effectLst/>
@@ -1254,16 +1280,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>290510</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>71435</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1724024</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200024</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1588,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E2D784-53F5-4A62-8F14-E71D11A057E2}">
-  <dimension ref="B4:E14"/>
+  <dimension ref="C4:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1605,65 +1631,65 @@
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>10</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E7">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E9">
         <v>6</v>
@@ -1671,42 +1697,74 @@
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D10">
         <v>4</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>43105</v>
       </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>43136</v>
       </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>43164</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="D5:E14">
+    <sortCondition descending="1" ref="D5"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="271" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>